<commit_message>
update data so one to one match
</commit_message>
<xml_diff>
--- a/LoopConditional/radio_merger_data.xlsx
+++ b/LoopConditional/radio_merger_data.xlsx
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:XFD68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,34 +847,34 @@
         <v>2007</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>32.886575999999998</v>
+        <v>40.384990999999999</v>
       </c>
       <c r="E13">
-        <v>-96.769577999999996</v>
+        <v>-104.68062999999999</v>
       </c>
       <c r="F13">
-        <v>31.392779999999998</v>
+        <v>38.064413000000002</v>
       </c>
       <c r="G13">
-        <v>-94.850881999999999</v>
+        <v>-103.54521</v>
       </c>
       <c r="H13">
-        <v>788819.56</v>
+        <v>131469.93</v>
       </c>
       <c r="I13">
-        <v>57</v>
+        <v>200</v>
       </c>
       <c r="J13">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="K13">
-        <v>86771</v>
+        <v>18831</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -885,34 +885,34 @@
         <v>2007</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14">
-        <v>40.384990999999999</v>
+        <v>27.689785000000001</v>
       </c>
       <c r="E14">
-        <v>-104.68062999999999</v>
+        <v>-80.375726</v>
       </c>
       <c r="F14">
-        <v>38.064413000000002</v>
+        <v>35.624586000000001</v>
       </c>
       <c r="G14">
-        <v>-103.54521</v>
+        <v>-105.21642</v>
       </c>
       <c r="H14">
-        <v>131469.93</v>
+        <v>736231.59</v>
       </c>
       <c r="I14">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K14">
-        <v>18831</v>
+        <v>29393</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -923,34 +923,34 @@
         <v>2007</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15">
-        <v>27.689785000000001</v>
+        <v>34.722960999999998</v>
       </c>
       <c r="E15">
-        <v>-80.375726</v>
+        <v>-88.903623999999994</v>
       </c>
       <c r="F15">
-        <v>35.624586000000001</v>
+        <v>34.917560000000002</v>
       </c>
       <c r="G15">
-        <v>-105.21642</v>
+        <v>-88.247253000000001</v>
       </c>
       <c r="H15">
-        <v>736231.59</v>
+        <v>383892.19</v>
       </c>
       <c r="I15">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K15">
-        <v>29393</v>
+        <v>19593</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -961,34 +961,34 @@
         <v>2007</v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D16">
-        <v>27.689785000000001</v>
+        <v>34.224891999999997</v>
       </c>
       <c r="E16">
-        <v>-80.375726</v>
+        <v>-119.17749000000001</v>
       </c>
       <c r="F16">
-        <v>35.624586000000001</v>
+        <v>35.718305000000001</v>
       </c>
       <c r="G16">
-        <v>-105.21642</v>
+        <v>-120.87379</v>
       </c>
       <c r="H16">
-        <v>473291.74</v>
+        <v>1262111.3</v>
       </c>
       <c r="I16">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="J16">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="K16">
-        <v>29393</v>
+        <v>269637</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -999,34 +999,34 @@
         <v>2007</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17">
-        <v>34.722960999999998</v>
+        <v>40.872531000000002</v>
       </c>
       <c r="E17">
-        <v>-88.903623999999994</v>
+        <v>-98.521343000000002</v>
       </c>
       <c r="F17">
-        <v>34.917560000000002</v>
+        <v>41.210943999999998</v>
       </c>
       <c r="G17">
-        <v>-88.247253000000001</v>
+        <v>-103.68154</v>
       </c>
       <c r="H17">
-        <v>383892.19</v>
+        <v>141987.51999999999</v>
       </c>
       <c r="I17">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="J17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K17">
-        <v>19593</v>
+        <v>3821</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1037,34 +1037,34 @@
         <v>2007</v>
       </c>
       <c r="B18">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D18">
-        <v>34.224891999999997</v>
+        <v>33.876752000000003</v>
       </c>
       <c r="E18">
-        <v>-119.17749000000001</v>
+        <v>-84.329123999999993</v>
       </c>
       <c r="F18">
-        <v>35.718305000000001</v>
+        <v>33.127209000000001</v>
       </c>
       <c r="G18">
-        <v>-120.87379</v>
+        <v>-84.311262999999997</v>
       </c>
       <c r="H18">
-        <v>1262111.3</v>
+        <v>3575982</v>
       </c>
       <c r="I18">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="J18">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>269637</v>
+        <v>17869</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1075,34 +1075,34 @@
         <v>2007</v>
       </c>
       <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>33.786594000000001</v>
+      </c>
+      <c r="E19">
+        <v>-118.29866</v>
+      </c>
+      <c r="F19">
+        <v>33.846662999999999</v>
+      </c>
+      <c r="G19">
+        <v>-116.50528</v>
+      </c>
+      <c r="H19">
+        <v>18405790</v>
+      </c>
+      <c r="I19">
+        <v>13</v>
+      </c>
+      <c r="J19">
         <v>16</v>
       </c>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19">
-        <v>40.872531000000002</v>
-      </c>
-      <c r="E19">
-        <v>-98.521343000000002</v>
-      </c>
-      <c r="F19">
-        <v>41.210943999999998</v>
-      </c>
-      <c r="G19">
-        <v>-103.68154</v>
-      </c>
-      <c r="H19">
-        <v>141987.51999999999</v>
-      </c>
-      <c r="I19">
-        <v>58</v>
-      </c>
-      <c r="J19">
-        <v>10</v>
-      </c>
       <c r="K19">
-        <v>3821</v>
+        <v>2189641</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1113,34 +1113,34 @@
         <v>2007</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>33.876752000000003</v>
+        <v>44.061450999999998</v>
       </c>
       <c r="E20">
-        <v>-84.329123999999993</v>
+        <v>-94.003112000000002</v>
       </c>
       <c r="F20">
-        <v>33.127209000000001</v>
+        <v>44.181339000000001</v>
       </c>
       <c r="G20">
-        <v>-84.311262999999997</v>
+        <v>-93.836005999999998</v>
       </c>
       <c r="H20">
-        <v>3575982</v>
+        <v>3292007</v>
       </c>
       <c r="I20">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K20">
-        <v>17869</v>
+        <v>64013</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -1151,10 +1151,10 @@
         <v>2007</v>
       </c>
       <c r="B21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>33.786594000000001</v>
@@ -1163,22 +1163,22 @@
         <v>-118.29866</v>
       </c>
       <c r="F21">
-        <v>33.846662999999999</v>
+        <v>36.408622000000001</v>
       </c>
       <c r="G21">
-        <v>-116.50528</v>
+        <v>-119.62813</v>
       </c>
       <c r="H21">
-        <v>18405790</v>
+        <v>2313870.7000000002</v>
       </c>
       <c r="I21">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="J21">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="K21">
-        <v>2189641</v>
+        <v>152982</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1189,34 +1189,34 @@
         <v>2007</v>
       </c>
       <c r="B22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>44.061450999999998</v>
+        <v>37.666578999999999</v>
       </c>
       <c r="E22">
-        <v>-94.003112000000002</v>
+        <v>-97.435012</v>
       </c>
       <c r="F22">
-        <v>44.181339000000001</v>
+        <v>37.251486</v>
       </c>
       <c r="G22">
-        <v>-93.836005999999998</v>
+        <v>-96.743194000000003</v>
       </c>
       <c r="H22">
-        <v>3292007</v>
+        <v>631055.65</v>
       </c>
       <c r="I22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J22">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K22">
-        <v>64013</v>
+        <v>36311</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -1227,34 +1227,34 @@
         <v>2007</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C23">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D23">
-        <v>33.786594000000001</v>
+        <v>40.845050000000001</v>
       </c>
       <c r="E23">
-        <v>-118.29866</v>
+        <v>-96.698645999999997</v>
       </c>
       <c r="F23">
-        <v>36.408622000000001</v>
+        <v>42.250033000000002</v>
       </c>
       <c r="G23">
-        <v>-119.62813</v>
+        <v>-103.01125999999999</v>
       </c>
       <c r="H23">
-        <v>2313870.7000000002</v>
+        <v>378633.39</v>
       </c>
       <c r="I23">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="J23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K23">
-        <v>152982</v>
+        <v>11308</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -1265,34 +1265,34 @@
         <v>2007</v>
       </c>
       <c r="B24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D24">
-        <v>37.666578999999999</v>
+        <v>32.403111000000003</v>
       </c>
       <c r="E24">
-        <v>-97.435012</v>
+        <v>-88.658233999999993</v>
       </c>
       <c r="F24">
-        <v>37.251486</v>
+        <v>32.503070999999998</v>
       </c>
       <c r="G24">
-        <v>-96.743194000000003</v>
+        <v>-89.030930999999995</v>
       </c>
       <c r="H24">
-        <v>631055.65</v>
+        <v>893995.5</v>
       </c>
       <c r="I24">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
       <c r="K24">
-        <v>36311</v>
+        <v>21720</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -1303,34 +1303,34 @@
         <v>2007</v>
       </c>
       <c r="B25">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C25">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D25">
-        <v>40.845050000000001</v>
+        <v>48.704839</v>
       </c>
       <c r="E25">
-        <v>-96.698645999999997</v>
+        <v>-95.750382999999999</v>
       </c>
       <c r="F25">
-        <v>42.250033000000002</v>
+        <v>48.906401000000002</v>
       </c>
       <c r="G25">
-        <v>-103.01125999999999</v>
+        <v>-95.390933000000004</v>
       </c>
       <c r="H25">
-        <v>378633.39</v>
+        <v>399668.58</v>
       </c>
       <c r="I25">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25">
-        <v>11308</v>
+        <v>15629</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -1341,34 +1341,34 @@
         <v>2007</v>
       </c>
       <c r="B26">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C26">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>32.403111000000003</v>
+        <v>41.093763000000003</v>
       </c>
       <c r="E26">
-        <v>-88.658233999999993</v>
+        <v>-85.070712999999998</v>
       </c>
       <c r="F26">
-        <v>32.503070999999998</v>
+        <v>41.729101</v>
       </c>
       <c r="G26">
-        <v>-89.030930999999995</v>
+        <v>-84.896252000000004</v>
       </c>
       <c r="H26">
-        <v>893995.5</v>
+        <v>1840579</v>
       </c>
       <c r="I26">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K26">
-        <v>21720</v>
+        <v>34185</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -1379,34 +1379,34 @@
         <v>2007</v>
       </c>
       <c r="B27">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D27">
-        <v>48.704839</v>
+        <v>32.622225</v>
       </c>
       <c r="E27">
-        <v>-95.750382999999999</v>
+        <v>-104.43333</v>
       </c>
       <c r="F27">
-        <v>48.906401000000002</v>
+        <v>33.391365999999998</v>
       </c>
       <c r="G27">
-        <v>-95.390933000000004</v>
+        <v>-104.53681</v>
       </c>
       <c r="H27">
-        <v>399668.58</v>
+        <v>525879.71</v>
       </c>
       <c r="I27">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K27">
-        <v>15629</v>
+        <v>65645</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -1417,34 +1417,34 @@
         <v>2007</v>
       </c>
       <c r="B28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D28">
-        <v>41.093763000000003</v>
+        <v>35.990141999999999</v>
       </c>
       <c r="E28">
-        <v>-85.070712999999998</v>
+        <v>-83.962180000000004</v>
       </c>
       <c r="F28">
-        <v>41.729101</v>
+        <v>35.940506999999997</v>
       </c>
       <c r="G28">
-        <v>-84.896252000000004</v>
+        <v>-84.354363000000006</v>
       </c>
       <c r="H28">
-        <v>1840579</v>
+        <v>2524222.6</v>
       </c>
       <c r="I28">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K28">
-        <v>34185</v>
+        <v>54181</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1455,34 +1455,34 @@
         <v>2007</v>
       </c>
       <c r="B29">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C29">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D29">
-        <v>32.622225</v>
+        <v>33.842567000000003</v>
       </c>
       <c r="E29">
-        <v>-104.43333</v>
+        <v>-116.52800000000001</v>
       </c>
       <c r="F29">
-        <v>33.391365999999998</v>
+        <v>33.846662999999999</v>
       </c>
       <c r="G29">
-        <v>-104.53681</v>
+        <v>-116.50528</v>
       </c>
       <c r="H29">
-        <v>525879.71</v>
+        <v>7888195.5999999996</v>
       </c>
       <c r="I29">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="J29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K29">
-        <v>65645</v>
+        <v>2189641</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -1493,34 +1493,34 @@
         <v>2007</v>
       </c>
       <c r="B30">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D30">
-        <v>35.990141999999999</v>
+        <v>32.502833000000003</v>
       </c>
       <c r="E30">
-        <v>-83.962180000000004</v>
+        <v>-92.094583</v>
       </c>
       <c r="F30">
-        <v>35.940506999999997</v>
+        <v>32.518943</v>
       </c>
       <c r="G30">
-        <v>-84.354363000000006</v>
+        <v>-92.122591999999997</v>
       </c>
       <c r="H30">
-        <v>2524222.6</v>
+        <v>946583.47</v>
       </c>
       <c r="I30">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
       <c r="K30">
-        <v>54181</v>
+        <v>153720</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -1531,34 +1531,34 @@
         <v>2007</v>
       </c>
       <c r="B31">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D31">
-        <v>33.842567000000003</v>
+        <v>38.440061</v>
       </c>
       <c r="E31">
-        <v>-116.52800000000001</v>
+        <v>-122.7106</v>
       </c>
       <c r="F31">
-        <v>33.846662999999999</v>
+        <v>38.224088999999999</v>
       </c>
       <c r="G31">
-        <v>-116.50528</v>
+        <v>-122.43342</v>
       </c>
       <c r="H31">
-        <v>7888195.5999999996</v>
+        <v>3050102.3</v>
       </c>
       <c r="I31">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="J31">
         <v>2</v>
       </c>
       <c r="K31">
-        <v>2189641</v>
+        <v>483878</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -1569,34 +1569,34 @@
         <v>2007</v>
       </c>
       <c r="B32">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C32">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D32">
-        <v>32.502833000000003</v>
+        <v>47.573816000000001</v>
       </c>
       <c r="E32">
-        <v>-92.094583</v>
+        <v>-120.35187999999999</v>
       </c>
       <c r="F32">
-        <v>32.518943</v>
+        <v>48.215380000000003</v>
       </c>
       <c r="G32">
-        <v>-92.122591999999997</v>
+        <v>-118.96463</v>
       </c>
       <c r="H32">
-        <v>946583.47</v>
+        <v>262939.84999999998</v>
       </c>
       <c r="I32">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="J32">
         <v>1</v>
       </c>
       <c r="K32">
-        <v>153720</v>
+        <v>41120</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -1607,34 +1607,34 @@
         <v>2007</v>
       </c>
       <c r="B33">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C33">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D33">
-        <v>38.440061</v>
+        <v>41.819459000000002</v>
       </c>
       <c r="E33">
-        <v>-122.7106</v>
+        <v>-71.411500000000004</v>
       </c>
       <c r="F33">
-        <v>38.224088999999999</v>
+        <v>41.176425000000002</v>
       </c>
       <c r="G33">
-        <v>-122.43342</v>
+        <v>-71.579931000000002</v>
       </c>
       <c r="H33">
-        <v>3050102.3</v>
+        <v>2692504.1</v>
       </c>
       <c r="I33">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="J33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K33">
-        <v>483878</v>
+        <v>126979</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -1645,34 +1645,34 @@
         <v>2007</v>
       </c>
       <c r="B34">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C34">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D34">
-        <v>47.573816000000001</v>
+        <v>39.840809999999998</v>
       </c>
       <c r="E34">
-        <v>-120.35187999999999</v>
+        <v>-85.010441999999998</v>
       </c>
       <c r="F34">
-        <v>48.215380000000003</v>
+        <v>39.637829000000004</v>
       </c>
       <c r="G34">
-        <v>-118.96463</v>
+        <v>-85.370131000000001</v>
       </c>
       <c r="H34">
-        <v>262939.84999999998</v>
+        <v>1577639.1</v>
       </c>
       <c r="I34">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K34">
-        <v>41120</v>
+        <v>17392</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -1683,34 +1683,34 @@
         <v>2007</v>
       </c>
       <c r="B35">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C35">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D35">
-        <v>41.819459000000002</v>
+        <v>42.239933000000001</v>
       </c>
       <c r="E35">
-        <v>-71.411500000000004</v>
+        <v>-83.150823000000003</v>
       </c>
       <c r="F35">
-        <v>41.176425000000002</v>
+        <v>43.628078000000002</v>
       </c>
       <c r="G35">
-        <v>-71.579931000000002</v>
+        <v>-70.018443000000005</v>
       </c>
       <c r="H35">
-        <v>2692504.1</v>
+        <v>3681157.9</v>
       </c>
       <c r="I35">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="K35">
-        <v>126979</v>
+        <v>281674</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -1721,34 +1721,34 @@
         <v>2007</v>
       </c>
       <c r="B36">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C36">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D36">
-        <v>39.840809999999998</v>
+        <v>44.132294999999999</v>
       </c>
       <c r="E36">
-        <v>-85.010441999999998</v>
+        <v>-87.599030999999997</v>
       </c>
       <c r="F36">
-        <v>39.637829000000004</v>
+        <v>44.597932999999998</v>
       </c>
       <c r="G36">
-        <v>-85.370131000000001</v>
+        <v>-89.963224999999994</v>
       </c>
       <c r="H36">
-        <v>1577639.1</v>
+        <v>283975.03999999998</v>
       </c>
       <c r="I36">
-        <v>94</v>
+        <v>208</v>
       </c>
       <c r="J36">
         <v>3</v>
       </c>
       <c r="K36">
-        <v>17392</v>
+        <v>74749</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -1759,34 +1759,34 @@
         <v>2007</v>
       </c>
       <c r="B37">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C37">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D37">
-        <v>42.239933000000001</v>
+        <v>45.164861999999999</v>
       </c>
       <c r="E37">
-        <v>-83.150823000000003</v>
+        <v>-95.020123999999996</v>
       </c>
       <c r="F37">
-        <v>43.628078000000002</v>
+        <v>44.307161999999998</v>
       </c>
       <c r="G37">
-        <v>-70.018443000000005</v>
+        <v>-94.452213999999998</v>
       </c>
       <c r="H37">
-        <v>3681157.9</v>
+        <v>525879.71</v>
       </c>
       <c r="I37">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J37">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="K37">
-        <v>281674</v>
+        <v>25893</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -1797,34 +1797,34 @@
         <v>2007</v>
       </c>
       <c r="B38">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C38">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D38">
-        <v>44.132294999999999</v>
+        <v>32.781179000000002</v>
       </c>
       <c r="E38">
-        <v>-87.599030999999997</v>
+        <v>-96.790329</v>
       </c>
       <c r="F38">
-        <v>44.597932999999998</v>
+        <v>34.387467000000001</v>
       </c>
       <c r="G38">
-        <v>-89.963224999999994</v>
+        <v>-111.47033999999999</v>
       </c>
       <c r="H38">
-        <v>283975.03999999998</v>
+        <v>6783848.2000000002</v>
       </c>
       <c r="I38">
-        <v>208</v>
+        <v>73</v>
       </c>
       <c r="J38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K38">
-        <v>74749</v>
+        <v>53597</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -1835,34 +1835,34 @@
         <v>2007</v>
       </c>
       <c r="B39">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C39">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D39">
-        <v>45.164861999999999</v>
+        <v>34.298091999999997</v>
       </c>
       <c r="E39">
-        <v>-95.020123999999996</v>
+        <v>-110.03518</v>
       </c>
       <c r="F39">
-        <v>44.307161999999998</v>
+        <v>31.810338000000002</v>
       </c>
       <c r="G39">
-        <v>-94.452213999999998</v>
+        <v>-94.533708000000004</v>
       </c>
       <c r="H39">
-        <v>525879.71</v>
+        <v>420703.77</v>
       </c>
       <c r="I39">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39">
-        <v>25893</v>
+        <v>64524</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -1873,34 +1873,34 @@
         <v>2007</v>
       </c>
       <c r="B40">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C40">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D40">
-        <v>32.781179000000002</v>
+        <v>36.653255999999999</v>
       </c>
       <c r="E40">
-        <v>-96.790329</v>
+        <v>-93.056340000000006</v>
       </c>
       <c r="F40">
-        <v>34.387467000000001</v>
+        <v>37.372213000000002</v>
       </c>
       <c r="G40">
-        <v>-111.47033999999999</v>
+        <v>-92.419927999999999</v>
       </c>
       <c r="H40">
-        <v>6783848.2000000002</v>
+        <v>210351.88</v>
       </c>
       <c r="I40">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J40">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K40">
-        <v>53597</v>
+        <v>18815</v>
       </c>
       <c r="L40">
         <v>0</v>
@@ -1911,34 +1911,34 @@
         <v>2007</v>
       </c>
       <c r="B41">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C41">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D41">
-        <v>34.298091999999997</v>
+        <v>33.786594000000001</v>
       </c>
       <c r="E41">
-        <v>-110.03518</v>
+        <v>-118.29866</v>
       </c>
       <c r="F41">
-        <v>31.810338000000002</v>
+        <v>30.320606000000002</v>
       </c>
       <c r="G41">
-        <v>-94.533708000000004</v>
+        <v>-97.754546000000005</v>
       </c>
       <c r="H41">
-        <v>420703.77</v>
+        <v>21035188</v>
       </c>
       <c r="I41">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="J41">
         <v>0</v>
       </c>
       <c r="K41">
-        <v>64524</v>
+        <v>1024266</v>
       </c>
       <c r="L41">
         <v>0</v>
@@ -1949,34 +1949,34 @@
         <v>2007</v>
       </c>
       <c r="B42">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C42">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D42">
-        <v>36.653255999999999</v>
+        <v>30.551887000000001</v>
       </c>
       <c r="E42">
-        <v>-93.056340000000006</v>
+        <v>-88.185603</v>
       </c>
       <c r="F42">
-        <v>37.372213000000002</v>
+        <v>35.399453000000001</v>
       </c>
       <c r="G42">
-        <v>-92.419927999999999</v>
+        <v>-87.863507999999996</v>
       </c>
       <c r="H42">
-        <v>210351.88</v>
+        <v>1262111.3</v>
       </c>
       <c r="I42">
-        <v>75</v>
+        <v>228</v>
       </c>
       <c r="J42">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K42">
-        <v>18815</v>
+        <v>17021</v>
       </c>
       <c r="L42">
         <v>0</v>
@@ -1987,34 +1987,34 @@
         <v>2007</v>
       </c>
       <c r="B43">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C43">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D43">
-        <v>33.786594000000001</v>
+        <v>41.283366000000001</v>
       </c>
       <c r="E43">
-        <v>-118.29866</v>
+        <v>-92.662674999999993</v>
       </c>
       <c r="F43">
-        <v>30.320606000000002</v>
+        <v>41.066166000000003</v>
       </c>
       <c r="G43">
-        <v>-97.754546000000005</v>
+        <v>-92.762156000000004</v>
       </c>
       <c r="H43">
-        <v>21035188</v>
+        <v>168281.51</v>
       </c>
       <c r="I43">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43">
-        <v>1024266</v>
+        <v>7970</v>
       </c>
       <c r="L43">
         <v>0</v>
@@ -2025,34 +2025,34 @@
         <v>2007</v>
       </c>
       <c r="B44">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C44">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D44">
-        <v>30.551887000000001</v>
+        <v>38.824689999999997</v>
       </c>
       <c r="E44">
-        <v>-88.185603</v>
+        <v>-104.56202999999999</v>
       </c>
       <c r="F44">
-        <v>35.399453000000001</v>
+        <v>38.270870000000002</v>
       </c>
       <c r="G44">
-        <v>-87.863507999999996</v>
+        <v>-85.786112000000003</v>
       </c>
       <c r="H44">
-        <v>1262111.3</v>
+        <v>1051759.3999999999</v>
       </c>
       <c r="I44">
-        <v>228</v>
+        <v>89</v>
       </c>
       <c r="J44">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K44">
-        <v>17021</v>
+        <v>741096</v>
       </c>
       <c r="L44">
         <v>0</v>
@@ -2063,34 +2063,34 @@
         <v>2007</v>
       </c>
       <c r="B45">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C45">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D45">
-        <v>41.283366000000001</v>
+        <v>31.091784000000001</v>
       </c>
       <c r="E45">
-        <v>-92.662674999999993</v>
+        <v>-87.264039999999994</v>
       </c>
       <c r="F45">
-        <v>41.066166000000003</v>
+        <v>31.105533999999999</v>
       </c>
       <c r="G45">
-        <v>-92.762156000000004</v>
+        <v>-86.932436999999993</v>
       </c>
       <c r="H45">
-        <v>168281.51</v>
+        <v>1461945.6</v>
       </c>
       <c r="I45">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J45">
         <v>1</v>
       </c>
       <c r="K45">
-        <v>7970</v>
+        <v>38319</v>
       </c>
       <c r="L45">
         <v>0</v>
@@ -2101,34 +2101,34 @@
         <v>2007</v>
       </c>
       <c r="B46">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C46">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D46">
-        <v>38.824689999999997</v>
+        <v>39.328456000000003</v>
       </c>
       <c r="E46">
-        <v>-104.56202999999999</v>
+        <v>-76.599138999999994</v>
       </c>
       <c r="F46">
-        <v>38.270870000000002</v>
+        <v>38.379562</v>
       </c>
       <c r="G46">
-        <v>-85.786112000000003</v>
+        <v>-75.036063999999996</v>
       </c>
       <c r="H46">
-        <v>1051759.3999999999</v>
+        <v>1135900.2</v>
       </c>
       <c r="I46">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K46">
-        <v>741096</v>
+        <v>51454</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -2136,37 +2136,37 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B47">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="C47">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>31.091784000000001</v>
+        <v>40.369568999999998</v>
       </c>
       <c r="E47">
-        <v>-87.264039999999994</v>
+        <v>-80.043925000000002</v>
       </c>
       <c r="F47">
-        <v>31.105533999999999</v>
+        <v>41.052579000000001</v>
       </c>
       <c r="G47">
-        <v>-86.932436999999993</v>
+        <v>-77.683351000000002</v>
       </c>
       <c r="H47">
-        <v>1461945.6</v>
+        <v>1215732.1000000001</v>
       </c>
       <c r="I47">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="J47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K47">
-        <v>38319</v>
+        <v>153990</v>
       </c>
       <c r="L47">
         <v>0</v>
@@ -2174,37 +2174,37 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B48">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D48">
-        <v>39.328456000000003</v>
+        <v>44.752378999999998</v>
       </c>
       <c r="E48">
-        <v>-76.599138999999994</v>
+        <v>-87.625888000000003</v>
       </c>
       <c r="F48">
-        <v>38.379562</v>
+        <v>45.020679000000001</v>
       </c>
       <c r="G48">
-        <v>-75.036063999999996</v>
+        <v>-87.010079000000005</v>
       </c>
       <c r="H48">
-        <v>1135900.2</v>
+        <v>721840.96</v>
       </c>
       <c r="I48">
-        <v>79</v>
+        <v>288</v>
       </c>
       <c r="J48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K48">
-        <v>51454</v>
+        <v>27785</v>
       </c>
       <c r="L48">
         <v>0</v>
@@ -2215,34 +2215,34 @@
         <v>2008</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D49">
-        <v>40.369568999999998</v>
+        <v>32.96678</v>
       </c>
       <c r="E49">
-        <v>-80.043925000000002</v>
+        <v>-79.852834999999999</v>
       </c>
       <c r="F49">
-        <v>41.052579000000001</v>
+        <v>33.259483000000003</v>
       </c>
       <c r="G49">
-        <v>-77.683351000000002</v>
+        <v>-80.215357999999995</v>
       </c>
       <c r="H49">
-        <v>1215732.1000000001</v>
+        <v>1519665.2</v>
       </c>
       <c r="I49">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="J49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K49">
-        <v>153990</v>
+        <v>177843</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -2253,34 +2253,34 @@
         <v>2008</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D50">
-        <v>44.752378999999998</v>
+        <v>35.551538999999998</v>
       </c>
       <c r="E50">
-        <v>-87.625888000000003</v>
+        <v>-104.98564</v>
       </c>
       <c r="F50">
-        <v>45.020679000000001</v>
+        <v>35.624586000000001</v>
       </c>
       <c r="G50">
-        <v>-87.010079000000005</v>
+        <v>-105.21642</v>
       </c>
       <c r="H50">
-        <v>721840.96</v>
+        <v>607866.06999999995</v>
       </c>
       <c r="I50">
-        <v>288</v>
+        <v>43</v>
       </c>
       <c r="J50">
         <v>1</v>
       </c>
       <c r="K50">
-        <v>27785</v>
+        <v>29393</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -2291,34 +2291,34 @@
         <v>2008</v>
       </c>
       <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>41.631408</v>
+      </c>
+      <c r="E51">
+        <v>-108.96393</v>
+      </c>
+      <c r="F51">
+        <v>42.761600999999999</v>
+      </c>
+      <c r="G51">
+        <v>-105.38094</v>
+      </c>
+      <c r="H51">
+        <v>405244.05</v>
+      </c>
+      <c r="I51">
+        <v>43</v>
+      </c>
+      <c r="J51">
         <v>3</v>
       </c>
-      <c r="C51">
-        <v>3</v>
-      </c>
-      <c r="D51">
-        <v>32.96678</v>
-      </c>
-      <c r="E51">
-        <v>-79.852834999999999</v>
-      </c>
-      <c r="F51">
-        <v>33.259483000000003</v>
-      </c>
-      <c r="G51">
-        <v>-80.215357999999995</v>
-      </c>
-      <c r="H51">
-        <v>1519665.2</v>
-      </c>
-      <c r="I51">
-        <v>93</v>
-      </c>
-      <c r="J51">
-        <v>4</v>
-      </c>
       <c r="K51">
-        <v>177843</v>
+        <v>13833</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -2329,34 +2329,34 @@
         <v>2008</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D52">
-        <v>35.551538999999998</v>
+        <v>40.756095000000002</v>
       </c>
       <c r="E52">
-        <v>-104.98564</v>
+        <v>-111.90072000000001</v>
       </c>
       <c r="F52">
-        <v>35.624586000000001</v>
+        <v>34.259202000000002</v>
       </c>
       <c r="G52">
-        <v>-105.21642</v>
-      </c>
-      <c r="H52">
-        <v>607866.06999999995</v>
+        <v>-118.29188000000001</v>
+      </c>
+      <c r="H52" s="1">
+        <v>139300000</v>
       </c>
       <c r="I52">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>29393</v>
+        <v>9818605</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -2367,34 +2367,34 @@
         <v>2008</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D53">
-        <v>41.631408</v>
+        <v>30.335398000000001</v>
       </c>
       <c r="E53">
-        <v>-108.96393</v>
+        <v>-97.559807000000006</v>
       </c>
       <c r="F53">
-        <v>42.761600999999999</v>
+        <v>28.890628</v>
       </c>
       <c r="G53">
-        <v>-105.38094</v>
+        <v>-96.473365999999999</v>
       </c>
       <c r="H53">
-        <v>405244.05</v>
+        <v>886471.35</v>
       </c>
       <c r="I53">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="J53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K53">
-        <v>13833</v>
+        <v>14075</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -2405,34 +2405,34 @@
         <v>2008</v>
       </c>
       <c r="B54">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D54">
-        <v>40.756095000000002</v>
+        <v>30.395586000000002</v>
       </c>
       <c r="E54">
-        <v>-111.90072000000001</v>
+        <v>-97.750611000000006</v>
       </c>
       <c r="F54">
-        <v>34.259202000000002</v>
+        <v>28.890628</v>
       </c>
       <c r="G54">
-        <v>-118.29188000000001</v>
-      </c>
-      <c r="H54" s="1">
-        <v>139300000</v>
+        <v>-96.473365999999999</v>
+      </c>
+      <c r="H54">
+        <v>70917.707999999999</v>
       </c>
       <c r="I54">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54">
-        <v>9818605</v>
+        <v>14075</v>
       </c>
       <c r="L54">
         <v>0</v>
@@ -2443,34 +2443,34 @@
         <v>2008</v>
       </c>
       <c r="B55">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C55">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D55">
-        <v>30.335398000000001</v>
+        <v>25.558427999999999</v>
       </c>
       <c r="E55">
-        <v>-97.559807000000006</v>
+        <v>-80.458168000000001</v>
       </c>
       <c r="F55">
-        <v>28.890628</v>
+        <v>25.369354999999999</v>
       </c>
       <c r="G55">
-        <v>-96.473365999999999</v>
+        <v>-80.956061000000005</v>
       </c>
       <c r="H55">
-        <v>886471.35</v>
+        <v>2330153.2999999998</v>
       </c>
       <c r="I55">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="J55">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K55">
-        <v>14075</v>
+        <v>73090</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -2481,34 +2481,34 @@
         <v>2008</v>
       </c>
       <c r="B56">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C56">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D56">
-        <v>30.395586000000002</v>
+        <v>35.006675999999999</v>
       </c>
       <c r="E56">
-        <v>-97.750611000000006</v>
+        <v>-78.415414999999996</v>
       </c>
       <c r="F56">
-        <v>28.890628</v>
+        <v>35.118744999999997</v>
       </c>
       <c r="G56">
-        <v>-96.473365999999999</v>
+        <v>-77.905828</v>
       </c>
       <c r="H56">
-        <v>70917.707999999999</v>
+        <v>506555.06</v>
       </c>
       <c r="I56">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J56">
         <v>1</v>
       </c>
       <c r="K56">
-        <v>14075</v>
+        <v>58505</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -2519,37 +2519,37 @@
         <v>2008</v>
       </c>
       <c r="B57">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C57">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D57">
-        <v>25.558427999999999</v>
+        <v>40.764068000000002</v>
       </c>
       <c r="E57">
-        <v>-80.458168000000001</v>
+        <v>-73.973479999999995</v>
       </c>
       <c r="F57">
-        <v>25.369354999999999</v>
+        <v>40.407660999999997</v>
       </c>
       <c r="G57">
-        <v>-80.956061000000005</v>
+        <v>-111.8428</v>
       </c>
       <c r="H57">
-        <v>2330153.2999999998</v>
+        <v>26340863</v>
       </c>
       <c r="I57">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J57">
+        <v>170</v>
+      </c>
+      <c r="K57">
+        <v>516564</v>
+      </c>
+      <c r="L57">
         <v>1</v>
-      </c>
-      <c r="K57">
-        <v>73090</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -2557,37 +2557,37 @@
         <v>2008</v>
       </c>
       <c r="B58">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D58">
-        <v>35.006675999999999</v>
+        <v>29.431232000000001</v>
       </c>
       <c r="E58">
-        <v>-78.415414999999996</v>
+        <v>-98.427792999999994</v>
       </c>
       <c r="F58">
-        <v>35.118744999999997</v>
+        <v>40.913032000000001</v>
       </c>
       <c r="G58">
-        <v>-77.905828</v>
+        <v>-120.81796</v>
       </c>
       <c r="H58">
-        <v>506555.06</v>
+        <v>2786052.8</v>
       </c>
       <c r="I58">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="J58">
+        <v>591</v>
+      </c>
+      <c r="K58">
+        <v>34895</v>
+      </c>
+      <c r="L58">
         <v>1</v>
-      </c>
-      <c r="K58">
-        <v>58505</v>
-      </c>
-      <c r="L58">
-        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -2595,37 +2595,37 @@
         <v>2008</v>
       </c>
       <c r="B59">
+        <v>13</v>
+      </c>
+      <c r="C59">
+        <v>13</v>
+      </c>
+      <c r="D59">
+        <v>43.505369999999999</v>
+      </c>
+      <c r="E59">
+        <v>-110.78653</v>
+      </c>
+      <c r="F59">
+        <v>42.867516000000002</v>
+      </c>
+      <c r="G59">
+        <v>-110.90257</v>
+      </c>
+      <c r="H59">
+        <v>476161.76</v>
+      </c>
+      <c r="I59">
+        <v>58</v>
+      </c>
+      <c r="J59">
         <v>11</v>
       </c>
-      <c r="C59">
-        <v>11</v>
-      </c>
-      <c r="D59">
-        <v>40.764068000000002</v>
-      </c>
-      <c r="E59">
-        <v>-73.973479999999995</v>
-      </c>
-      <c r="F59">
-        <v>40.407660999999997</v>
-      </c>
-      <c r="G59">
-        <v>-111.8428</v>
-      </c>
-      <c r="H59">
-        <v>26340863</v>
-      </c>
-      <c r="I59">
-        <v>37</v>
-      </c>
-      <c r="J59">
-        <v>170</v>
-      </c>
       <c r="K59">
-        <v>516564</v>
+        <v>18106</v>
       </c>
       <c r="L59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -2633,37 +2633,37 @@
         <v>2008</v>
       </c>
       <c r="B60">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C60">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D60">
-        <v>29.431232000000001</v>
+        <v>36.132607</v>
       </c>
       <c r="E60">
-        <v>-98.427792999999994</v>
+        <v>-86.803747999999999</v>
       </c>
       <c r="F60">
-        <v>40.913032000000001</v>
+        <v>32.466645999999997</v>
       </c>
       <c r="G60">
-        <v>-120.81796</v>
+        <v>-90.822827000000004</v>
       </c>
       <c r="H60">
-        <v>2786052.8</v>
+        <v>911799.11</v>
       </c>
       <c r="I60">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="J60">
-        <v>591</v>
+        <v>5</v>
       </c>
       <c r="K60">
-        <v>34895</v>
+        <v>48773</v>
       </c>
       <c r="L60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -2671,34 +2671,34 @@
         <v>2008</v>
       </c>
       <c r="B61">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C61">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D61">
-        <v>43.505369999999999</v>
+        <v>38.819794999999999</v>
       </c>
       <c r="E61">
-        <v>-110.78653</v>
+        <v>-121.27744</v>
       </c>
       <c r="F61">
-        <v>42.867516000000002</v>
+        <v>44.093972999999998</v>
       </c>
       <c r="G61">
-        <v>-110.90257</v>
+        <v>-70.228497000000004</v>
       </c>
       <c r="H61">
-        <v>476161.76</v>
+        <v>1013110.1</v>
       </c>
       <c r="I61">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J61">
-        <v>11</v>
+        <v>263</v>
       </c>
       <c r="K61">
-        <v>18106</v>
+        <v>107702</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -2709,34 +2709,34 @@
         <v>2008</v>
       </c>
       <c r="B62">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C62">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D62">
-        <v>36.132607</v>
+        <v>39.494115000000001</v>
       </c>
       <c r="E62">
-        <v>-86.803747999999999</v>
+        <v>-80.221282000000002</v>
       </c>
       <c r="F62">
-        <v>32.466645999999997</v>
+        <v>39.634464000000001</v>
       </c>
       <c r="G62">
-        <v>-90.822827000000004</v>
+        <v>-79.953342000000006</v>
       </c>
       <c r="H62">
-        <v>911799.11</v>
+        <v>759832.59</v>
       </c>
       <c r="I62">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="J62">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K62">
-        <v>48773</v>
+        <v>96189</v>
       </c>
       <c r="L62">
         <v>0</v>
@@ -2747,34 +2747,34 @@
         <v>2008</v>
       </c>
       <c r="B63">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C63">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D63">
-        <v>38.819794999999999</v>
+        <v>41.015219000000002</v>
       </c>
       <c r="E63">
-        <v>-121.27744</v>
+        <v>-83.664786000000007</v>
       </c>
       <c r="F63">
-        <v>44.093972999999998</v>
+        <v>41.114285000000002</v>
       </c>
       <c r="G63">
-        <v>-70.228497000000004</v>
+        <v>-83.981460999999996</v>
       </c>
       <c r="H63">
-        <v>1013110.1</v>
+        <v>506555.06</v>
       </c>
       <c r="I63">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J63">
-        <v>263</v>
+        <v>6</v>
       </c>
       <c r="K63">
-        <v>107702</v>
+        <v>34499</v>
       </c>
       <c r="L63">
         <v>0</v>
@@ -2785,34 +2785,34 @@
         <v>2008</v>
       </c>
       <c r="B64">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C64">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D64">
-        <v>39.494115000000001</v>
+        <v>32.886575999999998</v>
       </c>
       <c r="E64">
-        <v>-80.221282000000002</v>
+        <v>-96.769577999999996</v>
       </c>
       <c r="F64">
-        <v>39.634464000000001</v>
+        <v>42.994622</v>
       </c>
       <c r="G64">
-        <v>-79.953342000000006</v>
+        <v>-112.41538</v>
       </c>
       <c r="H64">
-        <v>759832.59</v>
+        <v>1104290</v>
       </c>
       <c r="I64">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="J64">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="K64">
-        <v>96189</v>
+        <v>82839</v>
       </c>
       <c r="L64">
         <v>0</v>
@@ -2823,34 +2823,34 @@
         <v>2008</v>
       </c>
       <c r="B65">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C65">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D65">
-        <v>41.015219000000002</v>
+        <v>27.824369999999998</v>
       </c>
       <c r="E65">
-        <v>-83.664786000000007</v>
+        <v>-97.584067000000005</v>
       </c>
       <c r="F65">
-        <v>41.114285000000002</v>
+        <v>33.626612000000002</v>
       </c>
       <c r="G65">
-        <v>-83.981460999999996</v>
+        <v>-101.83614</v>
       </c>
       <c r="H65">
-        <v>506555.06</v>
+        <v>455899.55</v>
       </c>
       <c r="I65">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="J65">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K65">
-        <v>34499</v>
+        <v>278831</v>
       </c>
       <c r="L65">
         <v>0</v>
@@ -2861,34 +2861,34 @@
         <v>2008</v>
       </c>
       <c r="B66">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C66">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D66">
-        <v>32.886575999999998</v>
+        <v>36.514384</v>
       </c>
       <c r="E66">
-        <v>-96.769577999999996</v>
+        <v>-82.547614999999993</v>
       </c>
       <c r="F66">
-        <v>42.994622</v>
+        <v>36.642026999999999</v>
       </c>
       <c r="G66">
-        <v>-112.41538</v>
+        <v>-82.586849999999998</v>
       </c>
       <c r="H66">
-        <v>1104290</v>
+        <v>273539.73</v>
       </c>
       <c r="I66">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="J66">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="K66">
-        <v>82839</v>
+        <v>23177</v>
       </c>
       <c r="L66">
         <v>0</v>
@@ -2899,34 +2899,34 @@
         <v>2008</v>
       </c>
       <c r="B67">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C67">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D67">
-        <v>27.824369999999998</v>
+        <v>33.381338999999997</v>
       </c>
       <c r="E67">
-        <v>-97.584067000000005</v>
+        <v>-86.704571000000001</v>
       </c>
       <c r="F67">
-        <v>33.626612000000002</v>
+        <v>33.906677999999999</v>
       </c>
       <c r="G67">
-        <v>-101.83614</v>
+        <v>-86.457200999999998</v>
       </c>
       <c r="H67">
-        <v>455899.55</v>
+        <v>1114421.1000000001</v>
       </c>
       <c r="I67">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="J67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K67">
-        <v>278831</v>
+        <v>57322</v>
       </c>
       <c r="L67">
         <v>0</v>
@@ -2937,34 +2937,34 @@
         <v>2008</v>
       </c>
       <c r="B68">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C68">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D68">
-        <v>36.514384</v>
+        <v>31.160148</v>
       </c>
       <c r="E68">
-        <v>-82.547614999999993</v>
+        <v>-85.322984000000005</v>
       </c>
       <c r="F68">
-        <v>36.642026999999999</v>
+        <v>31.553014000000001</v>
       </c>
       <c r="G68">
-        <v>-82.586849999999998</v>
+        <v>-86.043093999999996</v>
       </c>
       <c r="H68">
-        <v>273539.73</v>
+        <v>1114421.1000000001</v>
       </c>
       <c r="I68">
-        <v>137</v>
+        <v>47</v>
       </c>
       <c r="J68">
         <v>4</v>
       </c>
       <c r="K68">
-        <v>23177</v>
+        <v>49948</v>
       </c>
       <c r="L68">
         <v>0</v>
@@ -2975,34 +2975,34 @@
         <v>2008</v>
       </c>
       <c r="B69">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C69">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D69">
-        <v>33.381338999999997</v>
+        <v>32.800027999999998</v>
       </c>
       <c r="E69">
-        <v>-86.704571000000001</v>
+        <v>-96.781228999999996</v>
       </c>
       <c r="F69">
-        <v>33.906677999999999</v>
+        <v>34.387467000000001</v>
       </c>
       <c r="G69">
-        <v>-86.457200999999998</v>
+        <v>-111.47033999999999</v>
       </c>
       <c r="H69">
-        <v>1114421.1000000001</v>
+        <v>3039330.4</v>
       </c>
       <c r="I69">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="J69">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K69">
-        <v>57322</v>
+        <v>53597</v>
       </c>
       <c r="L69">
         <v>0</v>
@@ -3013,34 +3013,34 @@
         <v>2008</v>
       </c>
       <c r="B70">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C70">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D70">
-        <v>31.160148</v>
+        <v>40.745527000000003</v>
       </c>
       <c r="E70">
-        <v>-85.322984000000005</v>
+        <v>-73.978448999999998</v>
       </c>
       <c r="F70">
-        <v>31.553014000000001</v>
+        <v>32.464011999999997</v>
       </c>
       <c r="G70">
-        <v>-86.043093999999996</v>
+        <v>-89.839596999999998</v>
       </c>
       <c r="H70">
-        <v>1114421.1000000001</v>
+        <v>709177.08</v>
       </c>
       <c r="I70">
-        <v>47</v>
+        <v>316</v>
       </c>
       <c r="J70">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K70">
-        <v>49948</v>
+        <v>141617</v>
       </c>
       <c r="L70">
         <v>0</v>
@@ -3051,34 +3051,34 @@
         <v>2008</v>
       </c>
       <c r="B71">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C71">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D71">
-        <v>32.800027999999998</v>
+        <v>32.980974000000003</v>
       </c>
       <c r="E71">
-        <v>-96.781228999999996</v>
+        <v>-96.604557</v>
       </c>
       <c r="F71">
-        <v>34.387467000000001</v>
+        <v>32.983837000000001</v>
       </c>
       <c r="G71">
-        <v>-111.47033999999999</v>
+        <v>-95.000063999999995</v>
       </c>
       <c r="H71">
-        <v>3039330.4</v>
+        <v>57240.722000000002</v>
       </c>
       <c r="I71">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="J71">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K71">
-        <v>53597</v>
+        <v>12401</v>
       </c>
       <c r="L71">
         <v>0</v>
@@ -3089,34 +3089,34 @@
         <v>2008</v>
       </c>
       <c r="B72">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C72">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D72">
-        <v>40.745527000000003</v>
+        <v>35.476393000000002</v>
       </c>
       <c r="E72">
-        <v>-73.978448999999998</v>
+        <v>-93.369461000000001</v>
       </c>
       <c r="F72">
-        <v>32.464011999999997</v>
+        <v>35.614922999999997</v>
       </c>
       <c r="G72">
-        <v>-89.839596999999998</v>
+        <v>-93.464316999999994</v>
       </c>
       <c r="H72">
-        <v>709177.08</v>
+        <v>455393</v>
       </c>
       <c r="I72">
-        <v>316</v>
+        <v>57</v>
       </c>
       <c r="J72">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K72">
-        <v>141617</v>
+        <v>25540</v>
       </c>
       <c r="L72">
         <v>0</v>
@@ -3127,34 +3127,34 @@
         <v>2008</v>
       </c>
       <c r="B73">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C73">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D73">
-        <v>32.980974000000003</v>
+        <v>42.092486999999998</v>
       </c>
       <c r="E73">
-        <v>-96.604557</v>
+        <v>-88.116129000000001</v>
       </c>
       <c r="F73">
-        <v>32.983837000000001</v>
+        <v>37.579287000000001</v>
       </c>
       <c r="G73">
-        <v>-95.000063999999995</v>
+        <v>-99.257751999999996</v>
       </c>
       <c r="H73">
-        <v>57240.722000000002</v>
+        <v>392073.62</v>
       </c>
       <c r="I73">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="J73">
         <v>1</v>
       </c>
       <c r="K73">
-        <v>12401</v>
+        <v>2553</v>
       </c>
       <c r="L73">
         <v>0</v>
@@ -3165,34 +3165,34 @@
         <v>2008</v>
       </c>
       <c r="B74">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C74">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D74">
-        <v>35.476393000000002</v>
+        <v>36.242370999999999</v>
       </c>
       <c r="E74">
-        <v>-93.369461000000001</v>
+        <v>-116.16057000000001</v>
       </c>
       <c r="F74">
-        <v>35.614922999999997</v>
+        <v>38.741523000000001</v>
       </c>
       <c r="G74">
-        <v>-93.464316999999994</v>
+        <v>-116.85614</v>
       </c>
       <c r="H74">
-        <v>455393</v>
+        <v>607866.06999999995</v>
       </c>
       <c r="I74">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="J74">
         <v>1</v>
       </c>
       <c r="K74">
-        <v>25540</v>
+        <v>43946</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -3203,34 +3203,34 @@
         <v>2008</v>
       </c>
       <c r="B75">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C75">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D75">
-        <v>42.092486999999998</v>
+        <v>29.83399</v>
       </c>
       <c r="E75">
-        <v>-88.116129000000001</v>
+        <v>-95.434241</v>
       </c>
       <c r="F75">
-        <v>37.579287000000001</v>
+        <v>42.906590000000001</v>
       </c>
       <c r="G75">
-        <v>-99.257751999999996</v>
+        <v>-100.99312999999999</v>
       </c>
       <c r="H75">
-        <v>392073.62</v>
+        <v>1043503.4</v>
       </c>
       <c r="I75">
-        <v>90</v>
+        <v>232</v>
       </c>
       <c r="J75">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K75">
-        <v>2553</v>
+        <v>5713</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -3241,34 +3241,34 @@
         <v>2008</v>
       </c>
       <c r="B76">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C76">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D76">
-        <v>36.242370999999999</v>
+        <v>41.362112000000003</v>
       </c>
       <c r="E76">
-        <v>-116.16057000000001</v>
+        <v>-78.726237999999995</v>
       </c>
       <c r="F76">
-        <v>38.741523000000001</v>
+        <v>41.577990999999997</v>
       </c>
       <c r="G76">
-        <v>-116.85614</v>
+        <v>-78.676456999999999</v>
       </c>
       <c r="H76">
-        <v>607866.06999999995</v>
+        <v>1246125.3999999999</v>
       </c>
       <c r="I76">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="J76">
         <v>1</v>
       </c>
       <c r="K76">
-        <v>43946</v>
+        <v>31946</v>
       </c>
       <c r="L76">
         <v>0</v>
@@ -3279,34 +3279,34 @@
         <v>2008</v>
       </c>
       <c r="B77">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C77">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D77">
-        <v>29.83399</v>
+        <v>33.786594000000001</v>
       </c>
       <c r="E77">
-        <v>-95.434241</v>
+        <v>-118.29866</v>
       </c>
       <c r="F77">
-        <v>42.906590000000001</v>
+        <v>33.749037999999999</v>
       </c>
       <c r="G77">
-        <v>-100.99312999999999</v>
+        <v>-111.66853</v>
       </c>
       <c r="H77">
-        <v>1043503.4</v>
+        <v>15196652</v>
       </c>
       <c r="I77">
-        <v>232</v>
+        <v>388</v>
       </c>
       <c r="J77">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K77">
-        <v>5713</v>
+        <v>3817117</v>
       </c>
       <c r="L77">
         <v>0</v>
@@ -3317,34 +3317,34 @@
         <v>2008</v>
       </c>
       <c r="B78">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C78">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D78">
-        <v>41.362112000000003</v>
+        <v>32.759436999999998</v>
       </c>
       <c r="E78">
-        <v>-78.726237999999995</v>
+        <v>-97.245611999999994</v>
       </c>
       <c r="F78">
-        <v>41.577990999999997</v>
+        <v>33.282110000000003</v>
       </c>
       <c r="G78">
-        <v>-78.676456999999999</v>
+        <v>-98.166258999999997</v>
       </c>
       <c r="H78">
-        <v>1246125.3999999999</v>
+        <v>709177.08</v>
       </c>
       <c r="I78">
-        <v>43</v>
+        <v>372</v>
       </c>
       <c r="J78">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K78">
-        <v>31946</v>
+        <v>9044</v>
       </c>
       <c r="L78">
         <v>0</v>
@@ -3355,34 +3355,34 @@
         <v>2008</v>
       </c>
       <c r="B79">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C79">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D79">
-        <v>33.786594000000001</v>
+        <v>36.729049000000003</v>
       </c>
       <c r="E79">
-        <v>-118.29866</v>
+        <v>-119.77153</v>
       </c>
       <c r="F79">
-        <v>33.749037999999999</v>
+        <v>36.738722000000003</v>
       </c>
       <c r="G79">
-        <v>-111.66853</v>
+        <v>-119.79443000000001</v>
       </c>
       <c r="H79">
-        <v>15196652</v>
+        <v>4660306.5</v>
       </c>
       <c r="I79">
-        <v>388</v>
+        <v>82</v>
       </c>
       <c r="J79">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K79">
-        <v>3817117</v>
+        <v>930450</v>
       </c>
       <c r="L79">
         <v>0</v>
@@ -3393,34 +3393,34 @@
         <v>2008</v>
       </c>
       <c r="B80">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C80">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D80">
-        <v>32.759436999999998</v>
+        <v>43.626131999999998</v>
       </c>
       <c r="E80">
-        <v>-97.245611999999994</v>
+        <v>-84.338030000000003</v>
       </c>
       <c r="F80">
-        <v>33.282110000000003</v>
+        <v>43.770319999999998</v>
       </c>
       <c r="G80">
-        <v>-98.166258999999997</v>
+        <v>-83.790625000000006</v>
       </c>
       <c r="H80">
-        <v>709177.08</v>
+        <v>329260.78999999998</v>
       </c>
       <c r="I80">
-        <v>372</v>
+        <v>77</v>
       </c>
       <c r="J80">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K80">
-        <v>9044</v>
+        <v>107771</v>
       </c>
       <c r="L80">
         <v>0</v>
@@ -3431,34 +3431,34 @@
         <v>2008</v>
       </c>
       <c r="B81">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C81">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D81">
-        <v>36.729049000000003</v>
+        <v>26.362566000000001</v>
       </c>
       <c r="E81">
-        <v>-119.77153</v>
+        <v>-81.818279000000004</v>
       </c>
       <c r="F81">
-        <v>36.738722000000003</v>
+        <v>36.485697000000002</v>
       </c>
       <c r="G81">
-        <v>-119.79443000000001</v>
+        <v>-84.113335000000006</v>
       </c>
       <c r="H81">
-        <v>4660306.5</v>
+        <v>861143.6</v>
       </c>
       <c r="I81">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J81">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K81">
-        <v>930450</v>
+        <v>40716</v>
       </c>
       <c r="L81">
         <v>0</v>
@@ -3469,34 +3469,34 @@
         <v>2008</v>
       </c>
       <c r="B82">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C82">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D82">
-        <v>43.626131999999998</v>
+        <v>32.811767000000003</v>
       </c>
       <c r="E82">
-        <v>-84.338030000000003</v>
+        <v>-83.565009000000003</v>
       </c>
       <c r="F82">
-        <v>43.770319999999998</v>
+        <v>32.856256000000002</v>
       </c>
       <c r="G82">
-        <v>-83.790625000000006</v>
+        <v>-83.188732000000002</v>
       </c>
       <c r="H82">
-        <v>329260.78999999998</v>
+        <v>1013110.1</v>
       </c>
       <c r="I82">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="J82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K82">
-        <v>107771</v>
+        <v>9563</v>
       </c>
       <c r="L82">
         <v>0</v>
@@ -3507,34 +3507,34 @@
         <v>2008</v>
       </c>
       <c r="B83">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C83">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D83">
-        <v>26.362566000000001</v>
+        <v>40.343625000000003</v>
       </c>
       <c r="E83">
-        <v>-81.818279000000004</v>
+        <v>-74.693952999999993</v>
       </c>
       <c r="F83">
-        <v>36.485697000000002</v>
+        <v>40.335591999999998</v>
       </c>
       <c r="G83">
-        <v>-84.113335000000006</v>
+        <v>-75.924700999999999</v>
       </c>
       <c r="H83">
-        <v>861143.6</v>
+        <v>22288423</v>
       </c>
       <c r="I83">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J83">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="K83">
-        <v>40716</v>
+        <v>411442</v>
       </c>
       <c r="L83">
         <v>0</v>
@@ -3545,34 +3545,34 @@
         <v>2008</v>
       </c>
       <c r="B84">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C84">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D84">
-        <v>32.811767000000003</v>
+        <v>32.436064000000002</v>
       </c>
       <c r="E84">
-        <v>-83.565009000000003</v>
+        <v>-90.137309999999999</v>
       </c>
       <c r="F84">
-        <v>32.856256000000002</v>
+        <v>32.374577000000002</v>
       </c>
       <c r="G84">
-        <v>-83.188732000000002</v>
+        <v>-90.133598000000006</v>
       </c>
       <c r="H84">
-        <v>1013110.1</v>
+        <v>3849818.4</v>
       </c>
       <c r="I84">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="J84">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K84">
-        <v>9563</v>
+        <v>245285</v>
       </c>
       <c r="L84">
         <v>0</v>
@@ -3583,34 +3583,34 @@
         <v>2008</v>
       </c>
       <c r="B85">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C85">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D85">
-        <v>40.343625000000003</v>
+        <v>40.262591</v>
       </c>
       <c r="E85">
-        <v>-74.693952999999993</v>
+        <v>-103.84765</v>
       </c>
       <c r="F85">
-        <v>40.335591999999998</v>
+        <v>40.901494999999997</v>
       </c>
       <c r="G85">
-        <v>-75.924700999999999</v>
+        <v>-102.99932</v>
       </c>
       <c r="H85">
-        <v>22288423</v>
+        <v>177294.27</v>
       </c>
       <c r="I85">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="J85">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K85">
-        <v>411442</v>
+        <v>22709</v>
       </c>
       <c r="L85">
         <v>0</v>
@@ -3621,34 +3621,34 @@
         <v>2008</v>
       </c>
       <c r="B86">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C86">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D86">
-        <v>32.436064000000002</v>
+        <v>41.060195999999998</v>
       </c>
       <c r="E86">
-        <v>-90.137309999999999</v>
+        <v>-73.544477000000001</v>
       </c>
       <c r="F86">
-        <v>32.374577000000002</v>
+        <v>33.894717999999997</v>
       </c>
       <c r="G86">
-        <v>-90.133598000000006</v>
+        <v>-78.306633000000005</v>
       </c>
       <c r="H86">
-        <v>3849818.4</v>
+        <v>4052440.5</v>
       </c>
       <c r="I86">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="J86">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="K86">
-        <v>245285</v>
+        <v>107431</v>
       </c>
       <c r="L86">
         <v>0</v>
@@ -3659,34 +3659,34 @@
         <v>2008</v>
       </c>
       <c r="B87">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C87">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D87">
-        <v>40.262591</v>
+        <v>27.963895999999998</v>
       </c>
       <c r="E87">
-        <v>-103.84765</v>
+        <v>-81.917603999999997</v>
       </c>
       <c r="F87">
-        <v>40.901494999999997</v>
+        <v>32.774425999999998</v>
       </c>
       <c r="G87">
-        <v>-102.99932</v>
+        <v>-79.939904999999996</v>
       </c>
       <c r="H87">
-        <v>177294.27</v>
+        <v>2330153.2999999998</v>
       </c>
       <c r="I87">
-        <v>57</v>
+        <v>372</v>
       </c>
       <c r="J87">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K87">
-        <v>22709</v>
+        <v>350209</v>
       </c>
       <c r="L87">
         <v>0</v>
@@ -3697,34 +3697,34 @@
         <v>2008</v>
       </c>
       <c r="B88">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C88">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D88">
-        <v>41.060195999999998</v>
+        <v>41.766950000000001</v>
       </c>
       <c r="E88">
-        <v>-73.544477000000001</v>
+        <v>-111.88508</v>
       </c>
       <c r="F88">
-        <v>33.894717999999997</v>
+        <v>43.376891999999998</v>
       </c>
       <c r="G88">
-        <v>-78.306633000000005</v>
+        <v>-112.1223</v>
       </c>
       <c r="H88">
-        <v>4052440.5</v>
+        <v>1114421.1000000001</v>
       </c>
       <c r="I88">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="J88">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="K88">
-        <v>107431</v>
+        <v>45607</v>
       </c>
       <c r="L88">
         <v>0</v>
@@ -3735,34 +3735,34 @@
         <v>2008</v>
       </c>
       <c r="B89">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C89">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D89">
-        <v>27.963895999999998</v>
+        <v>41.079982999999999</v>
       </c>
       <c r="E89">
-        <v>-81.917603999999997</v>
+        <v>-73.654471999999998</v>
       </c>
       <c r="F89">
-        <v>32.774425999999998</v>
+        <v>34.153095</v>
       </c>
       <c r="G89">
-        <v>-79.939904999999996</v>
+        <v>-77.789996000000002</v>
       </c>
       <c r="H89">
-        <v>2330153.2999999998</v>
+        <v>1013110.1</v>
       </c>
       <c r="I89">
-        <v>372</v>
+        <v>284</v>
       </c>
       <c r="J89">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="K89">
-        <v>350209</v>
+        <v>202667</v>
       </c>
       <c r="L89">
         <v>0</v>
@@ -3773,34 +3773,34 @@
         <v>2008</v>
       </c>
       <c r="B90">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C90">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D90">
-        <v>41.766950000000001</v>
+        <v>46.925359999999998</v>
       </c>
       <c r="E90">
-        <v>-111.88508</v>
+        <v>-96.990615000000005</v>
       </c>
       <c r="F90">
-        <v>43.376891999999998</v>
+        <v>45.943305000000002</v>
       </c>
       <c r="G90">
-        <v>-112.1223</v>
+        <v>-97.113630000000001</v>
       </c>
       <c r="H90">
-        <v>1114421.1000000001</v>
+        <v>1995826.9</v>
       </c>
       <c r="I90">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="J90">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K90">
-        <v>45607</v>
+        <v>16321</v>
       </c>
       <c r="L90">
         <v>0</v>
@@ -3811,34 +3811,34 @@
         <v>2008</v>
       </c>
       <c r="B91">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C91">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D91">
-        <v>41.079982999999999</v>
+        <v>33.523355000000002</v>
       </c>
       <c r="E91">
-        <v>-73.654471999999998</v>
+        <v>-90.277569999999997</v>
       </c>
       <c r="F91">
-        <v>34.153095</v>
+        <v>35.810805999999999</v>
       </c>
       <c r="G91">
-        <v>-77.789996000000002</v>
+        <v>-106.68687</v>
       </c>
       <c r="H91">
-        <v>1013110.1</v>
+        <v>1418354.2</v>
       </c>
       <c r="I91">
-        <v>284</v>
+        <v>92</v>
       </c>
       <c r="J91">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K91">
-        <v>202667</v>
+        <v>131561</v>
       </c>
       <c r="L91">
         <v>0</v>
@@ -3849,34 +3849,34 @@
         <v>2008</v>
       </c>
       <c r="B92">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C92">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D92">
-        <v>46.925359999999998</v>
+        <v>33.792005000000003</v>
       </c>
       <c r="E92">
-        <v>-96.990615000000005</v>
+        <v>-84.442778000000004</v>
       </c>
       <c r="F92">
-        <v>45.943305000000002</v>
+        <v>34.945773000000003</v>
       </c>
       <c r="G92">
-        <v>-97.113630000000001</v>
+        <v>-84.752387999999996</v>
       </c>
       <c r="H92">
-        <v>1995826.9</v>
+        <v>3241952.4</v>
       </c>
       <c r="I92">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="J92">
         <v>2</v>
       </c>
       <c r="K92">
-        <v>16321</v>
+        <v>39628</v>
       </c>
       <c r="L92">
         <v>0</v>
@@ -3887,34 +3887,34 @@
         <v>2008</v>
       </c>
       <c r="B93">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C93">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D93">
-        <v>33.523355000000002</v>
+        <v>31.304165999999999</v>
       </c>
       <c r="E93">
-        <v>-90.277569999999997</v>
+        <v>-86.386398</v>
       </c>
       <c r="F93">
-        <v>35.810805999999999</v>
+        <v>31.428021999999999</v>
       </c>
       <c r="G93">
-        <v>-106.68687</v>
+        <v>-86.431838999999997</v>
       </c>
       <c r="H93">
-        <v>1418354.2</v>
+        <v>1266387.6000000001</v>
       </c>
       <c r="I93">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="J93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K93">
-        <v>131561</v>
+        <v>37765</v>
       </c>
       <c r="L93">
         <v>0</v>
@@ -3925,34 +3925,34 @@
         <v>2008</v>
       </c>
       <c r="B94">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C94">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D94">
-        <v>33.792005000000003</v>
+        <v>41.655797999999997</v>
       </c>
       <c r="E94">
-        <v>-84.442778000000004</v>
+        <v>-83.536833000000001</v>
       </c>
       <c r="F94">
-        <v>34.945773000000003</v>
+        <v>41.850493999999998</v>
       </c>
       <c r="G94">
-        <v>-84.752387999999996</v>
+        <v>-83.175596999999996</v>
       </c>
       <c r="H94">
-        <v>3241952.4</v>
+        <v>1013110.1</v>
       </c>
       <c r="I94">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="J94">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K94">
-        <v>39628</v>
+        <v>441815</v>
       </c>
       <c r="L94">
         <v>0</v>
@@ -3963,34 +3963,34 @@
         <v>2008</v>
       </c>
       <c r="B95">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C95">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D95">
-        <v>31.304165999999999</v>
+        <v>36.832324</v>
       </c>
       <c r="E95">
-        <v>-86.386398</v>
+        <v>-81.597841000000003</v>
       </c>
       <c r="F95">
-        <v>31.428021999999999</v>
+        <v>36.900900999999998</v>
       </c>
       <c r="G95">
-        <v>-86.431838999999997</v>
+        <v>-81.494808000000006</v>
       </c>
       <c r="H95">
-        <v>1266387.6000000001</v>
+        <v>506555.06</v>
       </c>
       <c r="I95">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="J95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K95">
-        <v>37765</v>
+        <v>32208</v>
       </c>
       <c r="L95">
         <v>0</v>
@@ -4001,34 +4001,34 @@
         <v>2008</v>
       </c>
       <c r="B96">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C96">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D96">
-        <v>41.655797999999997</v>
+        <v>38.824689999999997</v>
       </c>
       <c r="E96">
-        <v>-83.536833000000001</v>
+        <v>-104.56202999999999</v>
       </c>
       <c r="F96">
-        <v>41.850493999999998</v>
+        <v>38.270870000000002</v>
       </c>
       <c r="G96">
-        <v>-83.175596999999996</v>
+        <v>-85.786112000000003</v>
       </c>
       <c r="H96">
-        <v>1013110.1</v>
+        <v>3039330.4</v>
       </c>
       <c r="I96">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J96">
         <v>0</v>
       </c>
       <c r="K96">
-        <v>441815</v>
+        <v>741096</v>
       </c>
       <c r="L96">
         <v>0</v>
@@ -4039,34 +4039,34 @@
         <v>2008</v>
       </c>
       <c r="B97">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C97">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D97">
-        <v>36.832324</v>
+        <v>39.609596000000003</v>
       </c>
       <c r="E97">
-        <v>-81.597841000000003</v>
+        <v>-79.967623000000003</v>
       </c>
       <c r="F97">
-        <v>36.900900999999998</v>
+        <v>38.820973000000002</v>
       </c>
       <c r="G97">
-        <v>-81.494808000000006</v>
+        <v>-80.042884000000001</v>
       </c>
       <c r="H97">
-        <v>506555.06</v>
+        <v>1063765.6000000001</v>
       </c>
       <c r="I97">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="J97">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="K97">
-        <v>32208</v>
+        <v>29405</v>
       </c>
       <c r="L97">
         <v>0</v>
@@ -4077,34 +4077,34 @@
         <v>2008</v>
       </c>
       <c r="B98">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C98">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D98">
-        <v>38.824689999999997</v>
+        <v>35.294404999999998</v>
       </c>
       <c r="E98">
-        <v>-104.56202999999999</v>
+        <v>-118.90517</v>
       </c>
       <c r="F98">
-        <v>38.270870000000002</v>
+        <v>37.104785</v>
       </c>
       <c r="G98">
-        <v>-85.786112000000003</v>
+        <v>-107.91985</v>
       </c>
       <c r="H98">
-        <v>3039330.4</v>
+        <v>253277.53</v>
       </c>
       <c r="I98">
-        <v>98</v>
+        <v>164</v>
       </c>
       <c r="J98">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K98">
-        <v>741096</v>
+        <v>51334</v>
       </c>
       <c r="L98">
         <v>0</v>
@@ -4115,34 +4115,34 @@
         <v>2008</v>
       </c>
       <c r="B99">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C99">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D99">
-        <v>39.609596000000003</v>
+        <v>40.278497999999999</v>
       </c>
       <c r="E99">
-        <v>-79.967623000000003</v>
+        <v>-76.875207000000003</v>
       </c>
       <c r="F99">
-        <v>38.820973000000002</v>
+        <v>40.10772</v>
       </c>
       <c r="G99">
-        <v>-80.042884000000001</v>
+        <v>-77.782639000000003</v>
       </c>
       <c r="H99">
-        <v>1063765.6000000001</v>
+        <v>886471.35</v>
       </c>
       <c r="I99">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="J99">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="K99">
-        <v>29405</v>
+        <v>149618</v>
       </c>
       <c r="L99">
         <v>0</v>
@@ -4153,112 +4153,36 @@
         <v>2008</v>
       </c>
       <c r="B100">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C100">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D100">
-        <v>35.294404999999998</v>
+        <v>31.489241</v>
       </c>
       <c r="E100">
-        <v>-118.90517</v>
+        <v>-87.052003999999997</v>
       </c>
       <c r="F100">
-        <v>37.104785</v>
+        <v>31.745024999999998</v>
       </c>
       <c r="G100">
-        <v>-107.91985</v>
+        <v>-87.138810000000007</v>
       </c>
       <c r="H100">
         <v>253277.53</v>
       </c>
       <c r="I100">
-        <v>164</v>
+        <v>70</v>
       </c>
       <c r="J100">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K100">
-        <v>51334</v>
+        <v>23068</v>
       </c>
       <c r="L100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>2008</v>
-      </c>
-      <c r="B101">
-        <v>53</v>
-      </c>
-      <c r="C101">
-        <v>53</v>
-      </c>
-      <c r="D101">
-        <v>40.278497999999999</v>
-      </c>
-      <c r="E101">
-        <v>-76.875207000000003</v>
-      </c>
-      <c r="F101">
-        <v>40.10772</v>
-      </c>
-      <c r="G101">
-        <v>-77.782639000000003</v>
-      </c>
-      <c r="H101">
-        <v>886471.35</v>
-      </c>
-      <c r="I101">
-        <v>80</v>
-      </c>
-      <c r="J101">
-        <v>2</v>
-      </c>
-      <c r="K101">
-        <v>149618</v>
-      </c>
-      <c r="L101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>2008</v>
-      </c>
-      <c r="B102">
-        <v>54</v>
-      </c>
-      <c r="C102">
-        <v>54</v>
-      </c>
-      <c r="D102">
-        <v>31.489241</v>
-      </c>
-      <c r="E102">
-        <v>-87.052003999999997</v>
-      </c>
-      <c r="F102">
-        <v>31.745024999999998</v>
-      </c>
-      <c r="G102">
-        <v>-87.138810000000007</v>
-      </c>
-      <c r="H102">
-        <v>253277.53</v>
-      </c>
-      <c r="I102">
-        <v>70</v>
-      </c>
-      <c r="J102">
-        <v>1</v>
-      </c>
-      <c r="K102">
-        <v>23068</v>
-      </c>
-      <c r="L102">
         <v>0</v>
       </c>
     </row>

</xml_diff>